<commit_message>
Update report 3 and review log
</commit_message>
<xml_diff>
--- a/Design/Usecase Diagram/Review/Review Log v1.0.xlsx
+++ b/Design/Usecase Diagram/Review/Review Log v1.0.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="41">
   <si>
     <t>No.</t>
   </si>
@@ -138,8 +138,35 @@
     <t>1. Không hiểu phần đặc tả của Trigger, hãy Update lại.
 2. Cân nhắc về những Field read only, nếu chỉ cho cập nhật thông tin giờ làm việc của bác sỹ thì có chính đáng hay không.
 3. Nếu có thay đổi những Field read only thì phải cập nhật lại Exception case tương ứng với với use case Add Doctor
-4. Alternative screnario có 2 dòng trùng lắp
-5.  Sửa lỗi chính tả, diễn đạt và định dạng</t>
+4. Không hiểu rõ Action của Step 2 và Step 4 trong Main Scenario
+5. Alternative screnario có 2 dòng trùng lắp
+6.  Sửa lỗi chính tả, diễn đạt và định dạng</t>
+  </si>
+  <si>
+    <t>&lt;HU&gt;&lt;AD&gt; Update hospital information</t>
+  </si>
+  <si>
+    <t>1. Trigger nên ghi rõ là click vào button hoặc link gì, hoặc có hành dộng nào trước đó trong những Page khác để kích hoạt chức năng này
+2. Mới chỉ miêu tả flow chạy chính của Admin. Flow chạy của Hospital user vẫn chưa được thể hiện
+3. Alternative Scenario là một cách khác để thực hiện case này, chứ không phải trong case này có những chức năng optinal nào. Trong trường hợp cụ thể ở đây thì nên để flow chạy của Hospital user
+4. Các field trong phần Giới thiệu chung chưa được phân loại kiểu giao diện (Textbox, lable,...). Các list nên ghi rõ là dạng Table hay Drop down list
+5. Việc Update thông tin của bệnh viện sẽ có nhiều Field cần Update, nhưng không thấy phần đặc tả cho Exception và Error message.
+6. Sửa lỗi chính tả, diễn đạt và định dạng</t>
+  </si>
+  <si>
+    <t>&lt;HU&gt; Update account information</t>
+  </si>
+  <si>
+    <t>&lt;HU&gt; General use case v1.1</t>
+  </si>
+  <si>
+    <t>1. Chưa có case Change password và Reclaim forgotten password</t>
+  </si>
+  <si>
+    <t>1. Tách thành 2 case:
+&lt;HU&gt; Change Password
+&lt;HU&gt; Reclaim forgotten password
+2. Sửa lại use case diagram. Cho Change Password và Reclaim forgotten password kế thừa Update account information</t>
   </si>
 </sst>
 </file>
@@ -725,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,14 +1039,12 @@
       <c r="F11" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="23">
-        <v>41798</v>
-      </c>
+      <c r="G11" s="23"/>
       <c r="H11" s="25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="255" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>11</v>
       </c>
@@ -1038,42 +1063,84 @@
       <c r="F12" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="23">
-        <v>41798</v>
-      </c>
+      <c r="G12" s="23"/>
       <c r="H12" s="25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="18"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="18"/>
+    <row r="13" spans="1:8" ht="360" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>12</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="23">
+        <v>41798</v>
+      </c>
+      <c r="E13" s="23">
+        <v>41798</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="23">
+        <v>41798</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
+        <v>13</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="23">
+        <v>41798</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="23"/>
+      <c r="H14" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="23">
+        <v>41798</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="23"/>
+      <c r="H15" s="25" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
@@ -2927,7 +2994,7 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E199 E2:E10 H2:H199">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10 H2:H199 E14:E199">
       <formula1>"Lê Phước Việt, Nguyễn Xuân Sơn, Vũ Nhật Anh Khoa, Dương Thị Hoàng Anh"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F199">

</xml_diff>

<commit_message>
Update report 3 and Use case review log for every use case of AnhDTH
</commit_message>
<xml_diff>
--- a/Design/Usecase Diagram/Review/Review Log v1.0.xlsx
+++ b/Design/Usecase Diagram/Review/Review Log v1.0.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="48">
   <si>
     <t>No.</t>
   </si>
@@ -171,10 +171,6 @@
     <t>&lt;US&gt; Comment</t>
   </si>
   <si>
-    <t>1. Sửa lỗi chính tả, diện đạt và định dạng
-2. Add exception error message</t>
-  </si>
-  <si>
     <t>&lt;US&gt; Reply comment</t>
   </si>
   <si>
@@ -187,6 +183,18 @@
   </si>
   <si>
     <t>&lt;GU&gt; Make appointment online</t>
+  </si>
+  <si>
+    <t>1. Sửa lỗi chính tả, diễn đạt và định dạng
+2. Add exception error message</t>
+  </si>
+  <si>
+    <t>1. Sửa lỗi chính tả, diễn đạt và định dạng
+2. Cân nhắc việc bỏ Checkbox đặt lịch khám cho bản thân hoặc người thân
+3. Cân nhắc lại ở Post Condition là lịch hẹn được đưa trực tiếp vào Google Calendar hay phải xác nhận bằng tin nhắn sau đó mới đưa vào Calendar
+4. Sửa giao diện Field Năm sinh thành Ngày sinh và type giao diện thành Datetime picker
+5. Nên tìm regular expression cho Phone number
+6. Ngày hẹn và giờ hẹn là Required nhưng chưa định nghĩa error message trong phần Exception</t>
   </si>
 </sst>
 </file>
@@ -772,7 +780,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1170,7 +1180,7 @@
         <v>41</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D16" s="23">
         <v>41798</v>
@@ -1193,10 +1203,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D17" s="23">
         <v>41798</v>
@@ -1219,10 +1229,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18" s="23">
         <v>41798</v>
@@ -1240,19 +1250,31 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="285" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>18</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="18"/>
+        <v>45</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="23">
+        <v>41799</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="23">
+        <v>41799</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
@@ -3055,7 +3077,7 @@
       <c r="H199" s="19"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E198 H2:H198 E2:E9">
       <formula1>"Lê Phước Việt, Nguyễn Xuân Sơn, Vũ Nhật Anh Khoa, Dương Thị Hoàng Anh"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Update use case review log for AnhDTH
</commit_message>
<xml_diff>
--- a/Design/Usecase Diagram/Review/Review Log v1.0.xlsx
+++ b/Design/Usecase Diagram/Review/Review Log v1.0.xlsx
@@ -69,11 +69,6 @@
     <t>&lt;GU&gt; Login</t>
   </si>
   <si>
-    <t>1. Sửa lỗi chính tả, diễn đạt và định dạng.
-2. Sửa lại Post condition
-3. Không có Username trong Login mà chỉ có Email</t>
-  </si>
-  <si>
     <t>&lt;HU&gt;&lt;AD&gt; Upload Photo</t>
   </si>
   <si>
@@ -88,11 +83,6 @@
 2. Thêm Facility vào phần thêm mới bệnh viện cùng với Service.
 3. Sửa lại Altenative scenario
 4. Thêm Business rules</t>
-  </si>
-  <si>
-    <t>1. Case view hospital / clinic information ở Guest không có Extend, nhưng ở User lại có Extend. Hãy thống nhất trường hợp này trong cả 2 Diagrams.
-2. Bổ sung thêm Case Cancel Appointment Online cho Guest General Use Case.
-3. Bổ sung thêm Case Make Appointment và Cancel Appointment Online cho User General Use Case.</t>
   </si>
   <si>
     <t>1. User cũng có thể đặt Appointment Online. Vẽ thêm một Association từ User vào Make Appoint Online hoặc cho User kế thừa Guest.
@@ -193,8 +183,22 @@
 2. Cân nhắc việc bỏ Checkbox đặt lịch khám cho bản thân hoặc người thân
 3. Cân nhắc lại ở Post Condition là lịch hẹn được đưa trực tiếp vào Google Calendar hay phải xác nhận bằng tin nhắn sau đó mới đưa vào Calendar
 4. Sửa giao diện Field Năm sinh thành Ngày sinh và type giao diện thành Datetime picker
-5. Nên tìm regular expression cho Phone number
-6. Ngày hẹn và giờ hẹn là Required nhưng chưa định nghĩa error message trong phần Exception</t>
+5. Số điện thoại có error message báo regular expression sai nhưng không thấy định nghĩa regular expression cho số điện thoại
+6. Ngày hẹn và giờ hẹn là Required nhưng chưa định nghĩa error message trong phần Exception
+7. Nên suy nghĩ đến việc chọn giờ hẹn như thế nào để hợp lý và không bị Conflict với những giờ hẹn khác của một bác sỹ</t>
+  </si>
+  <si>
+    <t>1. Sửa lỗi chính tả, diễn đạt và định dạng.
+2. Sửa lại Pre  condition vì không chắc chắn rằng sẽ có trang web với tên www.timkiembenhvien.vn
+3. Sửa lại Post condition
+4. Không có Username trong Login mà chỉ có Email
+5. Email trong form đăng nhập của Facebook không cần phải miêu tả Regular expression</t>
+  </si>
+  <si>
+    <t>1. Case view hospital / clinic information ở Guest không có Extend, nhưng ở User lại có Extend. Hãy thống nhất trường hợp này trong cả 2 Diagrams.
+2. Bổ sung thêm Case Cancel Appointment Online cho Guest General Use Case.
+3. Bổ sung thêm Case Make Appointment và Cancel Appointment Online cho User General Use Case.
+4. Bổ sung thêm Case View Appointment</t>
   </si>
 </sst>
 </file>
@@ -391,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -472,6 +476,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -780,9 +787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -830,7 +835,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="23">
         <v>41798</v>
@@ -846,7 +851,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -854,7 +859,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="D3" s="23">
         <v>41798</v>
@@ -878,7 +883,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D4" s="23">
         <v>41798</v>
@@ -902,7 +907,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="23">
         <v>41798</v>
@@ -925,10 +930,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="23">
         <v>41798</v>
@@ -951,10 +956,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="23">
         <v>41798</v>
@@ -977,10 +982,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="23">
         <v>41798</v>
@@ -1003,10 +1008,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9" s="23">
         <v>41798</v>
@@ -1029,10 +1034,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D10" s="23">
         <v>41798</v>
@@ -1053,10 +1058,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D11" s="23">
         <v>41798</v>
@@ -1077,10 +1082,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D12" s="23">
         <v>41798</v>
@@ -1103,10 +1108,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D13" s="23">
         <v>41798</v>
@@ -1127,10 +1132,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D14" s="23">
         <v>41798</v>
@@ -1151,10 +1156,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D15" s="23">
         <v>41798</v>
@@ -1177,10 +1182,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D16" s="23">
         <v>41798</v>
@@ -1203,10 +1208,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D17" s="23">
         <v>41798</v>
@@ -1229,10 +1234,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D18" s="23">
         <v>41798</v>
@@ -1250,15 +1255,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="285" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="360" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>18</v>
       </c>
       <c r="B19" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="20" t="s">
         <v>45</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>47</v>
       </c>
       <c r="D19" s="23">
         <v>41799</v>
@@ -3094,7 +3099,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H200"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3134,7 +3141,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -3142,19 +3149,19 @@
         <v>16</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="D2" s="23">
-        <v>41798</v>
+        <v>41799</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="26" t="s">
-        <v>15</v>
+      <c r="F2" s="28" t="s">
+        <v>10</v>
       </c>
       <c r="G2" s="23">
-        <v>41798</v>
+        <v>41799</v>
       </c>
       <c r="H2" s="25" t="s">
         <v>9</v>
@@ -5141,12 +5148,15 @@
       <c r="H200" s="10"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F199">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F199">
       <formula1>"Assign, Cancel, In progress, Finished"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E199 H2:H199">
       <formula1>"Lê Phước Việt, Nguyễn Xuân Sơn, Vũ Nhật Anh Khoa, Dương Thị Hoàng Anh"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+      <formula1>"Assigned, Canceled, In progress, Finished"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
change status assigned to finish
</commit_message>
<xml_diff>
--- a/Design/Usecase Diagram/Review/Review Log v1.0.xlsx
+++ b/Design/Usecase Diagram/Review/Review Log v1.0.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -541,7 +541,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -576,7 +576,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -787,7 +787,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -844,9 +846,11 @@
         <v>9</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="23"/>
+        <v>15</v>
+      </c>
+      <c r="G2" s="23">
+        <v>41806</v>
+      </c>
       <c r="H2" s="25" t="s">
         <v>6</v>
       </c>
@@ -868,9 +872,11 @@
         <v>9</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="20"/>
+        <v>15</v>
+      </c>
+      <c r="G3" s="23">
+        <v>41806</v>
+      </c>
       <c r="H3" s="25" t="s">
         <v>6</v>
       </c>
@@ -892,9 +898,11 @@
         <v>9</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="20"/>
+        <v>15</v>
+      </c>
+      <c r="G4" s="23">
+        <v>41806</v>
+      </c>
       <c r="H4" s="25" t="s">
         <v>6</v>
       </c>
@@ -1046,9 +1054,11 @@
         <v>41798</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="23"/>
+        <v>15</v>
+      </c>
+      <c r="G10" s="23">
+        <v>41806</v>
+      </c>
       <c r="H10" s="25" t="s">
         <v>6</v>
       </c>
@@ -1070,9 +1080,11 @@
         <v>41798</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="23"/>
+        <v>15</v>
+      </c>
+      <c r="G11" s="23">
+        <v>41806</v>
+      </c>
       <c r="H11" s="25" t="s">
         <v>6</v>
       </c>
@@ -1094,7 +1106,7 @@
         <v>41798</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G12" s="23">
         <v>41798</v>
@@ -1120,9 +1132,11 @@
         <v>9</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="23"/>
+        <v>15</v>
+      </c>
+      <c r="G13" s="23">
+        <v>41806</v>
+      </c>
       <c r="H13" s="25" t="s">
         <v>6</v>
       </c>
@@ -1144,9 +1158,11 @@
         <v>9</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="23"/>
+        <v>15</v>
+      </c>
+      <c r="G14" s="23">
+        <v>41806</v>
+      </c>
       <c r="H14" s="25" t="s">
         <v>6</v>
       </c>
@@ -1272,10 +1288,10 @@
         <v>9</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G19" s="23">
-        <v>41799</v>
+        <v>41806</v>
       </c>
       <c r="H19" s="25" t="s">
         <v>6</v>

</xml_diff>